<commit_message>
Changes to ConnectionRules.xlsx, ModelValidation:         - creating validation rules for new Union feature
</commit_message>
<xml_diff>
--- a/terraer_project/others/ConnectionRules.xlsx
+++ b/terraer_project/others/ConnectionRules.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="36">
   <si>
     <t xml:space="preserve">Allowed Connections In TerraER Modeling</t>
   </si>
@@ -70,7 +70,7 @@
     <t xml:space="preserve">Key Attribute</t>
   </si>
   <si>
-    <t xml:space="preserve">Conjunction or Overlap Connection</t>
+    <t xml:space="preserve">Conjunction, Overlap or Union Connection</t>
   </si>
   <si>
     <t xml:space="preserve">COC</t>
@@ -122,6 +122,9 @@
   </si>
   <si>
     <t xml:space="preserve">Overlap</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Union</t>
   </si>
   <si>
     <t xml:space="preserve">U</t>
@@ -476,20 +479,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:I41"/>
+  <dimension ref="B1:I45"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F10" activeCellId="0" sqref="F10"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H8" activeCellId="0" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.0688259109312"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="18.1012145748988"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.1012145748988"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.1740890688259"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="18.2105263157895"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.3157894736842"/>
     <col collapsed="false" hidden="false" max="7" min="6" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="44.2388663967611"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="44.5627530364373"/>
     <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -896,11 +899,11 @@
       <c r="B27" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="C27" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="D27" s="19" t="s">
-        <v>32</v>
+      <c r="C27" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>34</v>
       </c>
       <c r="E27" s="5" t="s">
         <v>9</v>
@@ -914,7 +917,7 @@
         <v>20</v>
       </c>
       <c r="D28" s="19" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E28" s="5" t="s">
         <v>9</v>
@@ -924,11 +927,11 @@
       <c r="B29" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="C29" s="17" t="s">
-        <v>29</v>
+      <c r="C29" s="13" t="s">
+        <v>20</v>
       </c>
       <c r="D29" s="19" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E29" s="5" t="s">
         <v>9</v>
@@ -938,123 +941,123 @@
       <c r="B30" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="C30" s="17" t="s">
+      <c r="C30" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B31" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="C31" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="D30" s="19" t="s">
+      <c r="D31" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B32" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="C32" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="D32" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="E30" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="20" t="s">
+      <c r="E32" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B33" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="C33" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B34" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="C31" s="19" t="s">
+      <c r="C34" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="D31" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E31" s="21" t="s">
+      <c r="D34" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E34" s="21" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B35" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D35" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E35" s="21" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B36" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="C36" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="D36" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E36" s="21" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B37" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="C37" s="0" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="C32" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D32" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E32" s="21" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="C33" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="D33" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E33" s="21" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="C34" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D34" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="E34" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="C35" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D35" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="E35" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="C36" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D36" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="E36" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="C37" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="D37" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="E37" s="5" t="s">
-        <v>9</v>
+      <c r="D37" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E37" s="21" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="C38" s="13" t="s">
+      <c r="C38" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D38" s="13" t="s">
         <v>20</v>
-      </c>
-      <c r="D38" s="9" t="s">
-        <v>31</v>
       </c>
       <c r="E38" s="5" t="s">
         <v>9</v>
@@ -1064,11 +1067,11 @@
       <c r="B39" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="C39" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="D39" s="13" t="s">
-        <v>20</v>
+      <c r="C39" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D39" s="16" t="s">
+        <v>25</v>
       </c>
       <c r="E39" s="5" t="s">
         <v>9</v>
@@ -1078,11 +1081,11 @@
       <c r="B40" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="C40" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="D40" s="16" t="s">
-        <v>25</v>
+      <c r="C40" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D40" s="9" t="s">
+        <v>31</v>
       </c>
       <c r="E40" s="5" t="s">
         <v>9</v>
@@ -1092,13 +1095,69 @@
       <c r="B41" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="C41" s="17" t="s">
+      <c r="C41" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D41" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B42" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="C42" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D42" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E42" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B43" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="C43" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="D41" s="9" t="s">
+      <c r="D43" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="E43" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B44" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="C44" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="D44" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="E44" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B45" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="C45" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="D45" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="E41" s="5" t="s">
+      <c r="E45" s="5" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>